<commit_message>
Added missing crimp connector
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="BoardQty">'cost. '!$G$1</definedName>
-    <definedName name="digikey_part_data">'cost. '!$H$5:$L$14</definedName>
-    <definedName name="farnell_part_data">'cost. '!$M$5:$Q$14</definedName>
-    <definedName name="global_part_data">'cost. '!$A$5:$G$14</definedName>
-    <definedName name="mouser_part_data">'cost. '!$R$5:$V$14</definedName>
-    <definedName name="PURCHASE_DESCRIPTION">'cost. '!$G$17</definedName>
-    <definedName name="rs_part_data">'cost. '!$W$5:$AA$14</definedName>
+    <definedName name="digikey_part_data">'cost. '!$H$5:$L$15</definedName>
+    <definedName name="farnell_part_data">'cost. '!$M$5:$Q$15</definedName>
+    <definedName name="global_part_data">'cost. '!$A$5:$G$15</definedName>
+    <definedName name="mouser_part_data">'cost. '!$R$5:$V$15</definedName>
+    <definedName name="PURCHASE_DESCRIPTION">'cost. '!$G$18</definedName>
+    <definedName name="rs_part_data">'cost. '!$W$5:$AA$15</definedName>
     <definedName name="TotalCost">'cost. '!$G$3</definedName>
-    <definedName name="USD_GBP">'cost. '!$C$17</definedName>
+    <definedName name="USD_GBP">'cost. '!$C$18</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -938,6 +938,95 @@
       </text>
     </comment>
     <comment ref="J14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.10      $0.10
+    10   $0.06      $0.64
+    25   $0.05      $1.20
+    50   $0.04      $2.06
+   100   $0.04      $3.97
+   250   $0.03      $8.56
+   500   $0.03     $16.44
+  1000   $0.03     $28.77
+  2500   $0.03     $65.08
+  7000   $0.02    $172.62
+ 14000   $0.02    $306.88
+ 35000   $0.02    $695.45
+ 49000   $0.02    $906.50</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (GBP):
+  Qty  -  Unit£  -  Ext£
+================
+     1   £0.03      £0.03
+  7000   £0.03    £186.90
+ 35000   £0.02    £773.50
+ 70000   £0.02  £1,386.00
+140000   £0.02  £2,562.00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+  7000   $0.03    $196.00
+ 14000   $0.02    $350.00
+ 21000   $0.02    $462.00
+ 28000   $0.02    $588.00
+ 49000   $0.02  $1,029.00
+ 98000   $0.02  $2,058.00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (GBP):
+  Qty  -  Unit£  -  Ext£
+================
+   100   £0.04      £3.50
+  1000   £0.03     £28.00
+  3000   £0.02     £72.00
+  7500   £0.02    £135.00
+ 15000   £0.02    £270.00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -965,7 +1054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M14" authorId="0">
+    <comment ref="M15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -978,7 +1067,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O14" authorId="0">
+    <comment ref="O15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1001,7 +1090,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R14" authorId="0">
+    <comment ref="R15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1014,7 +1103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T14" authorId="0">
+    <comment ref="T15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1035,7 +1124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0">
+    <comment ref="F17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1048,7 +1137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0">
+    <comment ref="I17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1061,7 +1150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N16" authorId="0">
+    <comment ref="N17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1074,7 +1163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S16" authorId="0">
+    <comment ref="S17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1087,7 +1176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X16" authorId="0">
+    <comment ref="X17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1100,7 +1189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0">
+    <comment ref="F18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1118,7 +1207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -1198,7 +1287,7 @@
     <t>J615#1</t>
   </si>
   <si>
-    <t>Conn_01x04_Male - p1/2</t>
+    <t>Conn_01x04_Male - p1/3</t>
   </si>
   <si>
     <t>Molex_KK-396_A-41791-0004_1x04_P3.96mm_Vertical</t>
@@ -1210,12 +1299,21 @@
     <t>J615#2</t>
   </si>
   <si>
-    <t>Conn_01x04_Male - p2/2</t>
+    <t>Conn_01x04_Male - p2/3</t>
   </si>
   <si>
     <t>09-50-8041</t>
   </si>
   <si>
+    <t>J615#3</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Male - p3/3</t>
+  </si>
+  <si>
+    <t>08-52-0071</t>
+  </si>
+  <si>
     <t>L601-L606</t>
   </si>
   <si>
@@ -1252,7 +1350,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>2020-10-24T00:36:55 CEST</t>
+    <t>2020-10-24T00:40:30 CEST</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1267,7 +1365,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2020-10-24 00:37:01</t>
+    <t>2020-10-24 00:40:44</t>
   </si>
   <si>
     <t>Digi-Key</t>
@@ -1303,6 +1401,9 @@
     <t>WM2124-ND</t>
   </si>
   <si>
+    <t>WM2302CT-ND</t>
+  </si>
+  <si>
     <t>445-181486-6-ND</t>
   </si>
   <si>
@@ -1327,6 +1428,9 @@
     <t>2063781</t>
   </si>
   <si>
+    <t>1355931</t>
+  </si>
+  <si>
     <t>3386927</t>
   </si>
   <si>
@@ -1351,6 +1455,9 @@
     <t>53809508041</t>
   </si>
   <si>
+    <t>53808520071</t>
+  </si>
+  <si>
     <t>810TFM252012ALMAR15</t>
   </si>
   <si>
@@ -1367,6 +1474,9 @@
   </si>
   <si>
     <t>6795155</t>
+  </si>
+  <si>
+    <t>6706688</t>
   </si>
   <si>
     <t>KiCost® v.1.1.3</t>
@@ -1908,7 +2018,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
@@ -1950,13 +2060,13 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G1" s="3">
         <v>100</v>
@@ -1964,11 +2074,11 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G2" s="4">
         <f>TotalCost/BoardQty</f>
@@ -1977,57 +2087,57 @@
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G3" s="5">
-        <f>SUM(G7:G14)</f>
+        <f>SUM(G7:G15)</f>
         <v>0</v>
       </c>
       <c r="K3" s="5">
-        <f>SUM(K7:K14)</f>
+        <f>SUM(K7:K15)</f>
         <v>0</v>
       </c>
       <c r="L3" s="6">
-        <f>(COUNTA(K7:K14)&amp;" of "&amp;ROWS(K7:K14)&amp;" parts found"</f>
+        <f>(COUNTA(K7:K15)&amp;" of "&amp;ROWS(K7:K15)&amp;" parts found"</f>
         <v>0</v>
       </c>
       <c r="P3" s="5">
-        <f>SUM(P7:P14)</f>
+        <f>SUM(P7:P15)</f>
         <v>0</v>
       </c>
       <c r="Q3" s="6">
-        <f>(COUNTA(P7:P14)&amp;" of "&amp;ROWS(P7:P14)&amp;" parts found"</f>
+        <f>(COUNTA(P7:P15)&amp;" of "&amp;ROWS(P7:P15)&amp;" parts found"</f>
         <v>0</v>
       </c>
       <c r="U3" s="5">
-        <f>SUM(U7:U14)</f>
+        <f>SUM(U7:U15)</f>
         <v>0</v>
       </c>
       <c r="V3" s="6">
-        <f>(COUNTA(U7:U14)&amp;" of "&amp;ROWS(U7:U14)&amp;" parts found"</f>
+        <f>(COUNTA(U7:U15)&amp;" of "&amp;ROWS(U7:U15)&amp;" parts found"</f>
         <v>0</v>
       </c>
       <c r="Z3" s="5">
-        <f>SUM(Z7:Z14)</f>
+        <f>SUM(Z7:Z15)</f>
         <v>0</v>
       </c>
       <c r="AA3" s="6">
-        <f>(COUNTA(Z7:Z14)&amp;" of "&amp;ROWS(Z7:Z14)&amp;" parts found"</f>
+        <f>(COUNTA(Z7:Z15)&amp;" of "&amp;ROWS(Z7:Z15)&amp;" parts found"</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -2041,28 +2151,28 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="10" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="11" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
@@ -2092,10 +2202,10 @@
         <v>7</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>6</v>
@@ -2104,13 +2214,13 @@
         <v>7</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>6</v>
@@ -2119,13 +2229,13 @@
         <v>7</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="T6" s="12" t="s">
         <v>6</v>
@@ -2134,13 +2244,13 @@
         <v>7</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="X6" s="12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Y6" s="12" t="s">
         <v>6</v>
@@ -2149,7 +2259,7 @@
         <v>7</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -2189,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M7" s="13">
         <v>82</v>
@@ -2203,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R7" s="13">
         <v>774</v>
@@ -2217,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="V7" s="15" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -2257,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M8" s="13">
         <v>3</v>
@@ -2271,7 +2381,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="R8" s="13">
         <v>303</v>
@@ -2285,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="V8" s="15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -2314,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J9" s="14">
         <f>iferror(lookup(if(I9="",E9,I9),{0,1,10,50,100,500,1000,2500,5000},{0.0,0.57,0.402,0.3042,0.265,0.19628,0.16683,0.15702,0.1472}),"")</f>
@@ -2325,10 +2435,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O9" s="14">
         <f>iferror(USD_GBP*lookup(if(N9="",E9,N9),{0,1,1300},{0.0,0.126,0.126}),"")</f>
@@ -2339,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="R9" s="13">
         <v>1306</v>
@@ -2353,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -2393,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M10" s="13">
         <v>24816</v>
@@ -2407,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="R10" s="13">
         <v>18674</v>
@@ -2421,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="W10" s="13">
         <v>1975</v>
@@ -2435,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="15" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -2467,7 +2577,7 @@
         <v>25000</v>
       </c>
       <c r="AA11" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -2507,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M12" s="13">
         <v>9557</v>
@@ -2521,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="R12" s="13">
         <v>9704</v>
@@ -2535,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="W12" s="13">
         <v>2510</v>
@@ -2549,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="AA12" s="15" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -2589,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M13" s="13">
         <v>4766</v>
@@ -2603,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="R13" s="13">
         <v>16107</v>
@@ -2617,7 +2727,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="W13" s="13">
         <v>28550</v>
@@ -2631,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="AA13" s="15" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -2642,13 +2752,13 @@
         <v>33</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="E14" s="13">
-        <f>BoardQty*6</f>
+        <f>CEILING(BoardQty*(8)*1,1)</f>
         <v>0</v>
       </c>
       <c r="F14" s="14">
@@ -2660,10 +2770,10 @@
         <v>0</v>
       </c>
       <c r="H14" s="13">
-        <v>133</v>
+        <v>200220</v>
       </c>
       <c r="J14" s="14">
-        <f>iferror(lookup(if(I14="",E14,I14),{0,1,10,25,50,100,250,500,1000,3000,6000,15000,30000,75000},{0.0,0.73,0.642,0.5964,0.5046,0.4588,0.43124,0.38536,0.31195,0.2936,0.28443,0.27525,0.26608,0.2569}),"")</f>
+        <f>iferror(lookup(if(I14="",E14,I14),{0,1,10,25,50,100,250,500,1000,2500,7000,14000,35000,49000},{0.0,0.1,0.064,0.048,0.0412,0.0397,0.03424,0.03288,0.02877,0.02603,0.02466,0.02192,0.01987,0.0185}),"")</f>
         <v>0</v>
       </c>
       <c r="K14" s="14">
@@ -2671,13 +2781,13 @@
         <v>0</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="M14" s="13">
+        <v>11675</v>
       </c>
       <c r="O14" s="14">
-        <f>iferror(USD_GBP*lookup(if(N14="",E14,N14),{0,1,5,10,50,250,500,1500,3000,15000},{0.0,0.695,0.695,0.695,0.363,0.27,0.249,0.225,0.219,0.212}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(N14="",E14,N14),{0,1,7000,35000,70000,140000},{0.0,0.0346,0.0267,0.0221,0.0198,0.0183}),"")</f>
         <v>0</v>
       </c>
       <c r="P14" s="14">
@@ -2685,13 +2795,13 @@
         <v>0</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="R14" s="16" t="s">
-        <v>57</v>
+        <v>73</v>
+      </c>
+      <c r="R14" s="13">
+        <v>63000</v>
       </c>
       <c r="T14" s="14">
-        <f>iferror(lookup(if(S14="",E14,S14),{0,1,10,100,500,1000,3000},{0.0,0.81,0.635,0.527,0.442,0.358,0.28}),"")</f>
+        <f>iferror(lookup(if(S14="",E14,S14),{0,1,7000,14000,21000,28000,49000,98000},{0.0,0.028,0.028,0.025,0.022,0.021,0.021,0.021}),"")</f>
         <v>0</v>
       </c>
       <c r="U14" s="14">
@@ -2699,206 +2809,306 @@
         <v>0</v>
       </c>
       <c r="V14" s="15" t="s">
-        <v>77</v>
+        <v>82</v>
+      </c>
+      <c r="W14" s="13">
+        <v>38100</v>
+      </c>
+      <c r="Y14" s="14">
+        <f>iferror(USD_GBP*lookup(if(X14="",E14,X14),{0,1,100,1000,3000,7500,15000},{0.0,0.035,0.035,0.028,0.024,0.018,0.018}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="14">
+        <f>iferror(if(X14="",E14,X14)*Y14,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="15" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
-      <c r="B16" s="17" t="s">
+    <row r="15" spans="1:27">
+      <c r="A15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="E15" s="13">
+        <f>BoardQty*6</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="14">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <f>iferror(E15*F15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>133</v>
+      </c>
+      <c r="J15" s="14">
+        <f>iferror(lookup(if(I15="",E15,I15),{0,1,10,25,50,100,250,500,1000,3000,6000,15000,30000,75000},{0.0,0.73,0.642,0.5964,0.5046,0.4588,0.43124,0.38536,0.31195,0.2936,0.28443,0.27525,0.26608,0.2569}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="14">
+        <f>iferror(if(I15="",E15,I15)*J15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15" s="14">
+        <f>iferror(USD_GBP*lookup(if(N15="",E15,N15),{0,1,5,10,50,250,500,1500,3000,15000},{0.0,0.695,0.695,0.695,0.363,0.27,0.249,0.225,0.219,0.212}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="14">
+        <f>iferror(if(N15="",E15,N15)*O15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="T15" s="14">
+        <f>iferror(lookup(if(S15="",E15,S15),{0,1,10,100,500,1000,3000},{0.0,0.81,0.635,0.527,0.442,0.358,0.28}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="14">
+        <f>iferror(if(S15="",E15,S15)*T15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="B17" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="5">
         <f>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+3)))</f>
         <v>0</v>
       </c>
-      <c r="I16" s="6">
-        <f>IFERROR(IF(OR(I7:I14),COUNTIFS(I7:I14,"&gt;0",K7:K14,"&lt;&gt;")&amp;" of "&amp;(ROWS(K7:K14)-COUNTBLANK(K7:K14))&amp;" parts purchased",""),"")</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <f>SUMIF(I7:I14,"&gt;0",K7:K14)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="6">
-        <f>IFERROR(IF(OR(N7:N14),COUNTIFS(N7:N14,"&gt;0",P7:P14,"&lt;&gt;")&amp;" of "&amp;(ROWS(P7:P14)-COUNTBLANK(P7:P14))&amp;" parts purchased",""),"")</f>
-        <v>0</v>
-      </c>
-      <c r="P16" s="5">
-        <f>SUMIF(N7:N14,"&gt;0",P7:P14)</f>
-        <v>0</v>
-      </c>
-      <c r="S16" s="6">
-        <f>IFERROR(IF(OR(S7:S14),COUNTIFS(S7:S14,"&gt;0",U7:U14,"&lt;&gt;")&amp;" of "&amp;(ROWS(U7:U14)-COUNTBLANK(U7:U14))&amp;" parts purchased",""),"")</f>
-        <v>0</v>
-      </c>
-      <c r="U16" s="5">
-        <f>SUMIF(S7:S14,"&gt;0",U7:U14)</f>
-        <v>0</v>
-      </c>
-      <c r="X16" s="6">
-        <f>IFERROR(IF(OR(X7:X14),COUNTIFS(X7:X14,"&gt;0",Z7:Z14,"&lt;&gt;")&amp;" of "&amp;(ROWS(Z7:Z14)-COUNTBLANK(Z7:Z14))&amp;" parts purchased",""),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="5">
-        <f>SUMIF(X7:X14,"&gt;0",Z7:Z14)</f>
+      <c r="I17" s="6">
+        <f>IFERROR(IF(OR(I7:I15),COUNTIFS(I7:I15,"&gt;0",K7:K15,"&lt;&gt;")&amp;" of "&amp;(ROWS(K7:K15)-COUNTBLANK(K7:K15))&amp;" parts purchased",""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <f>SUMIF(I7:I15,"&gt;0",K7:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="6">
+        <f>IFERROR(IF(OR(N7:N15),COUNTIFS(N7:N15,"&gt;0",P7:P15,"&lt;&gt;")&amp;" of "&amp;(ROWS(P7:P15)-COUNTBLANK(P7:P15))&amp;" parts purchased",""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <f>SUMIF(N7:N15,"&gt;0",P7:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="6">
+        <f>IFERROR(IF(OR(S7:S15),COUNTIFS(S7:S15,"&gt;0",U7:U15,"&lt;&gt;")&amp;" of "&amp;(ROWS(U7:U15)-COUNTBLANK(U7:U15))&amp;" parts purchased",""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="5">
+        <f>SUMIF(S7:S15,"&gt;0",U7:U15)</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="6">
+        <f>IFERROR(IF(OR(X7:X15),COUNTIFS(X7:X15,"&gt;0",Z7:Z15,"&lt;&gt;")&amp;" of "&amp;(ROWS(Z7:Z15)-COUNTBLANK(Z7:Z15))&amp;" parts purchased",""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="5">
+        <f>SUMIF(X7:X15,"&gt;0",Z7:Z15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
-      <c r="B17" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17">
+    <row r="18" spans="1:26">
+      <c r="B18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18">
         <v>1.24582957619477</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17">
-        <f t="array" ref="I17">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <f t="array" ref="N17">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <f t="array" ref="S17">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <f t="array" ref="X17">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+      <c r="F18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18">
+        <f t="array" ref="I18">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f t="array" ref="N18">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="array" ref="S18">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <f t="array" ref="X18">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
-      <c r="I18">
-        <f t="array" ref="I18">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <f t="array" ref="N18">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <f t="array" ref="S18">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <f t="array" ref="X18">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="19" spans="1:26">
+      <c r="I19">
+        <f t="array" ref="I19">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f t="array" ref="N19">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="array" ref="S19">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <f t="array" ref="X19">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
-      <c r="A19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I19">
-        <f t="array" ref="I19">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <f t="array" ref="N19">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <f t="array" ref="S19">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <f t="array" ref="X19">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="20" spans="1:26">
+      <c r="A20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20">
+        <f t="array" ref="I20">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f t="array" ref="N20">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="array" ref="S20">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <f t="array" ref="X20">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
-      <c r="I20">
-        <f t="array" ref="I20">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <f t="array" ref="N20">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <f t="array" ref="S20">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <f t="array" ref="X20">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="21" spans="1:26">
+      <c r="I21">
+        <f t="array" ref="I21">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f t="array" ref="N21">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f t="array" ref="S21">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <f t="array" ref="X21">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
-      <c r="I21">
-        <f t="array" ref="I21">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <f t="array" ref="N21">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <f t="array" ref="S21">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <f t="array" ref="X21">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="22" spans="1:26">
+      <c r="I22">
+        <f t="array" ref="I22">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f t="array" ref="N22">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f t="array" ref="S22">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <f t="array" ref="X22">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
-      <c r="I22">
-        <f t="array" ref="I22">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f t="array" ref="N22">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <f t="array" ref="S22">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X22">
-        <f t="array" ref="X22">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="23" spans="1:26">
+      <c r="I23">
+        <f t="array" ref="I23">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="array" ref="N23">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f t="array" ref="S23">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <f t="array" ref="X23">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
-      <c r="I23">
-        <f t="array" ref="I23">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <f t="array" ref="N23">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <f t="array" ref="S23">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <f t="array" ref="X23">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="24" spans="1:26">
+      <c r="I24">
+        <f t="array" ref="I24">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="array" ref="N24">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <f t="array" ref="S24">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <f t="array" ref="X24">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
-      <c r="I24">
-        <f t="array" ref="I24">IFERROR(CONCATENATE(TEXT(INDEX(I7:I14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),"##0"),",",INDEX(L7:L14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(I7:I14),IF(I7:I14&gt;0,IF(L7:L14&lt;&gt;"",ROW(I7:I14)-MIN(ROW(I7:I14))+1))),ROW()-ROW(A$17)+1)),",",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <f t="array" ref="N24">IFERROR(CONCATENATE(INDEX(Q7:Q14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(N7:N14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(N7:N14),IF(N7:N14&gt;0,IF(Q7:Q14&lt;&gt;"",ROW(N7:N14)-MIN(ROW(N7:N14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <f t="array" ref="S24">IFERROR(CONCATENATE(INDEX(V7:V14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",TEXT(INDEX(S7:S14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(S7:S14),IF(S7:S14&gt;0,IF(V7:V14&lt;&gt;"",ROW(S7:S14)-MIN(ROW(S7:S14))+1))),ROW()-ROW(A$17)+1)),"|",";")," ","_")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <f t="array" ref="X24">IFERROR(CONCATENATE(INDEX(AA7:AA14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",TEXT(INDEX(X7:X14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A14,SMALL(IF(ISNUMBER(X7:X14),IF(X7:X14&gt;0,IF(AA7:AA14&lt;&gt;"",ROW(X7:X14)-MIN(ROW(X7:X14))+1))),ROW()-ROW(A$17)+1))," ",";")),"")</f>
+    <row r="25" spans="1:26">
+      <c r="I25">
+        <f t="array" ref="I25">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f t="array" ref="N25">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f t="array" ref="S25">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f t="array" ref="X25">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="I26">
+        <f t="array" ref="I26">IFERROR(CONCATENATE(TEXT(INDEX(I7:I15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),"##0"),",",INDEX(L7:L15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(I7:I15),IF(I7:I15&gt;0,IF(L7:L15&lt;&gt;"",ROW(I7:I15)-MIN(ROW(I7:I15))+1))),ROW()-ROW(A$18)+1)),",",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="array" ref="N26">IFERROR(CONCATENATE(INDEX(Q7:Q15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(N7:N15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(N7:N15),IF(N7:N15&gt;0,IF(Q7:Q15&lt;&gt;"",ROW(N7:N15)-MIN(ROW(N7:N15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f t="array" ref="S26">IFERROR(CONCATENATE(INDEX(V7:V15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",TEXT(INDEX(S7:S15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"##0"),"|",SUBSTITUTE(SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(S7:S15),IF(S7:S15&gt;0,IF(V7:V15&lt;&gt;"",ROW(S7:S15)-MIN(ROW(S7:S15))+1))),ROW()-ROW(A$18)+1)),"|",";")," ","_")),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f t="array" ref="X26">IFERROR(CONCATENATE(INDEX(AA7:AA15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",TEXT(INDEX(X7:X15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1)),"##0")," ",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A15,SMALL(IF(ISNUMBER(X7:X15),IF(X7:X15&gt;0,IF(AA7:AA15&lt;&gt;"",ROW(X7:X15)-MIN(ROW(X7:X15))+1))),ROW()-ROW(A$18)+1))," ",";")),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2980,6 +3190,20 @@
       <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+1)),0),IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+1)),0),IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0),IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+1)),0))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="expression" dxfId="0" priority="33">
+      <formula>AND(ISBLANK(D15),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+4))),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+4))),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+4))),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+4))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="34">
+      <formula>IF(SUM(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+0)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+0)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+0)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+0)))=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
+      <formula>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+0)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+0)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+0)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+0)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="36" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+1)),0),IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+1)),0),IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0),IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+1)),0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ISBLANK(D7),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+4))),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+4))),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+4))),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+4))))</formula>
@@ -3023,573 +3247,671 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="1" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="53" operator="lessThan">
       <formula>E10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="57" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="58" operator="lessThan">
       <formula>E12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="1" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="63" operator="lessThan">
       <formula>E13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="1" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="68" operator="lessThan">
       <formula>E14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="1" priority="72" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="73" operator="lessThan">
+      <formula>E15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="1" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="38" operator="lessThan">
       <formula>E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="1" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="43" operator="lessThan">
       <formula>E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="1" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="48" operator="lessThan">
       <formula>E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="1" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="54" operator="greaterThan">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="1" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="59" operator="greaterThan">
       <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="1" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="64" operator="greaterThan">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="1" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="69" operator="greaterThan">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="1" priority="74" operator="greaterThan">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="1" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="39" operator="greaterThan">
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="1" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="44" operator="greaterThan">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="1" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="49" operator="greaterThan">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="4" priority="52" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="56" operator="lessThanOrEqual">
       <formula>F10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="4" priority="57" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="61" operator="lessThanOrEqual">
       <formula>F12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="4" priority="62" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="66" operator="lessThanOrEqual">
       <formula>F13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="4" priority="67" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="71" operator="lessThanOrEqual">
       <formula>F14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="cellIs" dxfId="4" priority="76" operator="lessThanOrEqual">
+      <formula>F15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="4" priority="37" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="41" operator="lessThanOrEqual">
       <formula>F7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="4" priority="42" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="46" operator="lessThanOrEqual">
       <formula>F8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="4" priority="47" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="51" operator="lessThanOrEqual">
       <formula>F9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="4" priority="51" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="55" operator="lessThanOrEqual">
       <formula>G10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="4" priority="56" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="60" operator="lessThanOrEqual">
       <formula>G12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="4" priority="61" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="65" operator="lessThanOrEqual">
       <formula>G13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="4" priority="66" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="70" operator="lessThanOrEqual">
       <formula>G14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="cellIs" dxfId="4" priority="75" operator="lessThanOrEqual">
+      <formula>G15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="4" priority="36" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="40" operator="lessThanOrEqual">
       <formula>G7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="4" priority="41" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="45" operator="lessThanOrEqual">
       <formula>G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="4" priority="46" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="50" operator="lessThanOrEqual">
       <formula>G9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="1" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="93" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="85" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="94" operator="lessThan">
       <formula>E10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="1" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="99" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="100" operator="lessThan">
       <formula>E12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="1" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="104" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="96" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="105" operator="lessThan">
       <formula>E13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="1" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="109" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="110" operator="lessThan">
       <formula>E14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M15">
+    <cfRule type="cellIs" dxfId="1" priority="114" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="115" operator="lessThan">
+      <formula>E15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="1" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="77" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="78" operator="lessThan">
       <formula>E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="1" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="82" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="83" operator="lessThan">
       <formula>E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="1" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="87" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="88" operator="lessThan">
       <formula>E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="expression" dxfId="3" priority="86">
+    <cfRule type="expression" dxfId="3" priority="95">
       <formula>AND(N10&gt;0,N10&lt;5)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="87" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="96" operator="greaterThan">
       <formula>M10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="cellIs" dxfId="1" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="101" operator="greaterThan">
       <formula>M12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="1" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="106" operator="greaterThan">
       <formula>M13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="expression" dxfId="3" priority="102">
-      <formula>AND(N14&gt;0,N14&lt;5)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="111" operator="greaterThan">
       <formula>M14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="expression" dxfId="3" priority="116">
+      <formula>AND(N15&gt;0,N15&lt;5)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="117" operator="greaterThan">
+      <formula>M15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="cellIs" dxfId="1" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="79" operator="greaterThan">
       <formula>M7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="cellIs" dxfId="1" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="84" operator="greaterThan">
       <formula>M8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="expression" dxfId="3" priority="80">
+    <cfRule type="expression" dxfId="3" priority="89">
       <formula>AND(N9&gt;0,N9&lt;1300)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="90" operator="greaterThan">
       <formula>M9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10">
-    <cfRule type="cellIs" dxfId="4" priority="89" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="98" operator="lessThanOrEqual">
       <formula>F10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="cellIs" dxfId="4" priority="94" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="103" operator="lessThanOrEqual">
       <formula>F12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="cellIs" dxfId="4" priority="99" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="108" operator="lessThanOrEqual">
       <formula>F13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="cellIs" dxfId="4" priority="105" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="113" operator="lessThanOrEqual">
       <formula>F14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O15">
+    <cfRule type="cellIs" dxfId="4" priority="119" operator="lessThanOrEqual">
+      <formula>F15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="cellIs" dxfId="4" priority="72" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="81" operator="lessThanOrEqual">
       <formula>F7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="cellIs" dxfId="4" priority="77" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="86" operator="lessThanOrEqual">
       <formula>F8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="cellIs" dxfId="4" priority="83" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="92" operator="lessThanOrEqual">
       <formula>F9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="cellIs" dxfId="4" priority="88" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="97" operator="lessThanOrEqual">
       <formula>G10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="cellIs" dxfId="4" priority="93" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="102" operator="lessThanOrEqual">
       <formula>G12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="cellIs" dxfId="4" priority="98" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="107" operator="lessThanOrEqual">
       <formula>G13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="cellIs" dxfId="4" priority="104" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="112" operator="lessThanOrEqual">
       <formula>G14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P15">
+    <cfRule type="cellIs" dxfId="4" priority="118" operator="lessThanOrEqual">
+      <formula>G15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="cellIs" dxfId="4" priority="71" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="80" operator="lessThanOrEqual">
       <formula>G7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="cellIs" dxfId="4" priority="76" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="85" operator="lessThanOrEqual">
       <formula>G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="cellIs" dxfId="4" priority="82" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="91" operator="lessThanOrEqual">
       <formula>G9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="1" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="135" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="122" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="136" operator="lessThan">
       <formula>E10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R12">
-    <cfRule type="cellIs" dxfId="1" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="140" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="127" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="141" operator="lessThan">
       <formula>E12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R13">
-    <cfRule type="cellIs" dxfId="1" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="145" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="132" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="146" operator="lessThan">
       <formula>E13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14">
-    <cfRule type="cellIs" dxfId="1" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="150" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="151" operator="lessThan">
       <formula>E14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="cellIs" dxfId="1" priority="156" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="157" operator="lessThan">
+      <formula>E15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="1" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="120" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="121" operator="lessThan">
       <formula>E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="1" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="125" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="112" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="126" operator="lessThan">
       <formula>E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9">
-    <cfRule type="cellIs" dxfId="1" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="130" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="117" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="131" operator="lessThan">
       <formula>E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="1" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="137" operator="greaterThan">
       <formula>R10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12">
-    <cfRule type="cellIs" dxfId="1" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="142" operator="greaterThan">
       <formula>R12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13">
-    <cfRule type="cellIs" dxfId="1" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="147" operator="greaterThan">
       <formula>R13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="cellIs" dxfId="1" priority="138" operator="greaterThan">
+    <cfRule type="expression" dxfId="3" priority="152">
+      <formula>AND(S14&gt;0,S14&lt;7000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="153" operator="greaterThan">
       <formula>R14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S15">
+    <cfRule type="cellIs" dxfId="1" priority="158" operator="greaterThan">
+      <formula>R15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S7">
-    <cfRule type="cellIs" dxfId="1" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="122" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8">
-    <cfRule type="cellIs" dxfId="1" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="127" operator="greaterThan">
       <formula>R8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="1" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="132" operator="greaterThan">
       <formula>R9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T10">
-    <cfRule type="cellIs" dxfId="4" priority="125" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="139" operator="lessThanOrEqual">
       <formula>F10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T12">
-    <cfRule type="cellIs" dxfId="4" priority="130" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="144" operator="lessThanOrEqual">
       <formula>F12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T13">
-    <cfRule type="cellIs" dxfId="4" priority="135" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="149" operator="lessThanOrEqual">
       <formula>F13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="cellIs" dxfId="4" priority="140" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="155" operator="lessThanOrEqual">
       <formula>F14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="T15">
+    <cfRule type="cellIs" dxfId="4" priority="160" operator="lessThanOrEqual">
+      <formula>F15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="T7">
-    <cfRule type="cellIs" dxfId="4" priority="110" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="124" operator="lessThanOrEqual">
       <formula>F7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8">
-    <cfRule type="cellIs" dxfId="4" priority="115" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="129" operator="lessThanOrEqual">
       <formula>F8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9">
-    <cfRule type="cellIs" dxfId="4" priority="120" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="134" operator="lessThanOrEqual">
       <formula>F9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U10">
-    <cfRule type="cellIs" dxfId="4" priority="124" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="138" operator="lessThanOrEqual">
       <formula>G10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12">
-    <cfRule type="cellIs" dxfId="4" priority="129" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="143" operator="lessThanOrEqual">
       <formula>G12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13">
-    <cfRule type="cellIs" dxfId="4" priority="134" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="148" operator="lessThanOrEqual">
       <formula>G13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14">
-    <cfRule type="cellIs" dxfId="4" priority="139" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="154" operator="lessThanOrEqual">
       <formula>G14</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="U15">
+    <cfRule type="cellIs" dxfId="4" priority="159" operator="lessThanOrEqual">
+      <formula>G15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="U7">
-    <cfRule type="cellIs" dxfId="4" priority="109" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="123" operator="lessThanOrEqual">
       <formula>G7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8">
-    <cfRule type="cellIs" dxfId="4" priority="114" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="128" operator="lessThanOrEqual">
       <formula>G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U9">
-    <cfRule type="cellIs" dxfId="4" priority="119" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="133" operator="lessThanOrEqual">
       <formula>G9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10">
-    <cfRule type="cellIs" dxfId="1" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="161" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="142" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="162" operator="lessThan">
       <formula>E10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W12">
-    <cfRule type="cellIs" dxfId="1" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="167" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="148" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="168" operator="lessThan">
       <formula>E12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W13">
-    <cfRule type="cellIs" dxfId="1" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="173" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="154" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="174" operator="lessThan">
       <formula>E13</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="W14">
+    <cfRule type="cellIs" dxfId="1" priority="179" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="180" operator="lessThan">
+      <formula>E14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="X10">
-    <cfRule type="expression" dxfId="3" priority="143">
+    <cfRule type="expression" dxfId="3" priority="163">
       <formula>AND(X10&gt;0,X10&lt;25)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="164" operator="greaterThan">
       <formula>W10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12">
-    <cfRule type="expression" dxfId="3" priority="149">
+    <cfRule type="expression" dxfId="3" priority="169">
       <formula>AND(X12&gt;0,X12&lt;10)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="170" operator="greaterThan">
       <formula>W12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13">
-    <cfRule type="expression" dxfId="3" priority="155">
+    <cfRule type="expression" dxfId="3" priority="175">
       <formula>AND(X13&gt;0,X13&lt;10)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="176" operator="greaterThan">
       <formula>W13</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="X14">
+    <cfRule type="expression" dxfId="3" priority="181">
+      <formula>AND(X14&gt;0,X14&lt;100)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="182" operator="greaterThan">
+      <formula>W14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Y10">
-    <cfRule type="cellIs" dxfId="4" priority="146" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="166" operator="lessThanOrEqual">
       <formula>F10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y12">
-    <cfRule type="cellIs" dxfId="4" priority="152" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="172" operator="lessThanOrEqual">
       <formula>F12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y13">
-    <cfRule type="cellIs" dxfId="4" priority="158" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="178" operator="lessThanOrEqual">
       <formula>F13</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Y14">
+    <cfRule type="cellIs" dxfId="4" priority="184" operator="lessThanOrEqual">
+      <formula>F14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Z10">
-    <cfRule type="cellIs" dxfId="4" priority="145" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="165" operator="lessThanOrEqual">
       <formula>G10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z12">
-    <cfRule type="cellIs" dxfId="4" priority="151" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="171" operator="lessThanOrEqual">
       <formula>G12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z13">
-    <cfRule type="cellIs" dxfId="4" priority="157" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="177" operator="lessThanOrEqual">
       <formula>G13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z14">
+    <cfRule type="cellIs" dxfId="4" priority="183" operator="lessThanOrEqual">
+      <formula>G14</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3617,8 +3939,12 @@
     <hyperlink ref="L14" r:id="rId22"/>
     <hyperlink ref="Q14" r:id="rId23"/>
     <hyperlink ref="V14" r:id="rId24"/>
+    <hyperlink ref="AA14" r:id="rId25"/>
+    <hyperlink ref="L15" r:id="rId26"/>
+    <hyperlink ref="Q15" r:id="rId27"/>
+    <hyperlink ref="V15" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId25"/>
+  <legacyDrawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>